<commit_message>
Succesfuly Create Workbook and deleting it using Automatio
</commit_message>
<xml_diff>
--- a/Excel/AutomationExcel.xlsx
+++ b/Excel/AutomationExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\AAAAAAAANAUKA\AUTOIT\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{790F12C6-DD08-463E-AFD3-A58AD99BF664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{16AD7B2E-D4E2-4AA1-8B0A-40F1902A6C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33945" yWindow="2610" windowWidth="21600" windowHeight="12585" xr2:uid="{A328949B-AB75-48ED-8692-624CFDC20898}"/>
+    <workbookView xWindow="33945" yWindow="2610" windowWidth="21600" windowHeight="12585" xr2:uid="{8CFC025F-5558-4EC2-97F1-1D2661D63A64}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E7EE9E-987B-41A7-A3F8-9C745A01D7BE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE0C2B4-FF6C-478B-B420-5FF816B74759}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>